<commit_message>
final seeds and xlsx
</commit_message>
<xml_diff>
--- a/excel/alimentosClean3.xlsx
+++ b/excel/alimentosClean3.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
   <si>
-    <t>Nombre</t>
+    <t>nombre</t>
   </si>
   <si>
     <t>cantidad</t>
@@ -36,13 +36,13 @@
     <t>lipidos</t>
   </si>
   <si>
-    <t>hidratos de carbono</t>
+    <t>hidratos_de_carbono</t>
   </si>
   <si>
     <t>etanol</t>
   </si>
   <si>
-    <t>Composición en Equivalente</t>
+    <t>composicion_en_equivalente</t>
   </si>
   <si>
     <t>agua de fruta</t>
@@ -4091,7 +4091,9 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="22.8516" style="42" customWidth="1"/>
-    <col min="2" max="8" width="10.8516" style="42" customWidth="1"/>
+    <col min="2" max="6" width="10.8516" style="42" customWidth="1"/>
+    <col min="7" max="7" width="28.3203" style="42" customWidth="1"/>
+    <col min="8" max="8" width="10.8516" style="42" customWidth="1"/>
     <col min="9" max="9" width="25.1719" style="42" customWidth="1"/>
     <col min="10" max="16384" width="10.8516" style="42" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
added de connection to env, seeds, xlxs to english, created the models for 3 tables, seed them
</commit_message>
<xml_diff>
--- a/excel/alimentosClean3.xlsx
+++ b/excel/alimentosClean3.xlsx
@@ -16,33 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>unidad</t>
-  </si>
-  <si>
-    <t>Kcal</t>
-  </si>
-  <si>
-    <t>proteinas</t>
-  </si>
-  <si>
-    <t>lipidos</t>
-  </si>
-  <si>
-    <t>hidratos_de_carbono</t>
-  </si>
-  <si>
-    <t>etanol</t>
-  </si>
-  <si>
-    <t>composicion_en_equivalente</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>proteins</t>
+  </si>
+  <si>
+    <t>lipids</t>
+  </si>
+  <si>
+    <t>carbohydrates</t>
+  </si>
+  <si>
+    <t>equivalent_composition</t>
   </si>
   <si>
     <t>agua de fruta</t>
@@ -51,7 +48,7 @@
     <t>TAZA</t>
   </si>
   <si>
-    <t>-</t>
+    <t>0</t>
   </si>
   <si>
     <t>0.5 FRUTA</t>
@@ -123,6 +120,9 @@
     <t>alcohol con refresco</t>
   </si>
   <si>
+    <t>OZ</t>
+  </si>
+  <si>
     <t>3 AZUCAR</t>
   </si>
   <si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Sopas secas</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>Arroz y pastas</t>
@@ -674,7 +677,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -702,17 +705,11 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -725,6 +722,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -753,16 +753,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1924,16 +1918,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="22.8516" style="1" customWidth="1"/>
-    <col min="2" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.1719" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="2" max="7" width="10.8516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1719" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="92" customHeight="1">
@@ -1960,9 +1954,6 @@
       </c>
       <c r="H1" t="s" s="2">
         <v>7</v>
-      </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="2" ht="27" customHeight="1">
@@ -1974,71 +1965,68 @@
       <c r="F2" s="5"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
     </row>
     <row r="3" ht="12.7" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
       </c>
       <c r="C3" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7">
         <v>70</v>
       </c>
       <c r="E3" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="7">
         <v>17.5</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" t="s" s="8">
-        <v>12</v>
+      <c r="H3" t="s" s="8">
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="12.7" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="C4" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="7">
         <v>60</v>
       </c>
       <c r="E4" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="7">
         <v>15</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" t="s" s="8">
-        <v>14</v>
+      <c r="H4" t="s" s="8">
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="12.7" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="C5" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7">
         <v>52.5</v>
@@ -2047,52 +2035,50 @@
         <v>1</v>
       </c>
       <c r="F5" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="7">
         <v>12</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" t="s" s="8">
-        <v>16</v>
+      <c r="H5" t="s" s="8">
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="12.7" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="7">
         <v>120</v>
       </c>
       <c r="E6" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="7">
         <v>30</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" t="s" s="8">
-        <v>18</v>
+      <c r="H6" t="s" s="8">
+        <v>17</v>
       </c>
     </row>
     <row r="7" ht="12.7" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7">
         <v>2</v>
       </c>
       <c r="C7" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="7">
         <v>85</v>
@@ -2101,52 +2087,50 @@
         <v>2</v>
       </c>
       <c r="F7" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="7">
         <v>19</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" t="s" s="8">
+      <c r="H7" t="s" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="27" customHeight="1">
+      <c r="A8" t="s" s="9">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" ht="27" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>21</v>
-      </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
       <c r="C8" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="7">
         <v>160</v>
       </c>
       <c r="E8" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="7">
         <v>40</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" t="s" s="8">
+      <c r="H8" t="s" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="12.7" customHeight="1">
+      <c r="A9" t="s" s="9">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" ht="12.7" customHeight="1">
-      <c r="A9" t="s" s="10">
-        <v>23</v>
-      </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7">
         <v>150</v>
@@ -2160,20 +2144,19 @@
       <c r="G9" s="7">
         <v>12</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" t="s" s="8">
-        <v>24</v>
+      <c r="H9" t="s" s="8">
+        <v>23</v>
       </c>
     </row>
     <row r="10" ht="12.7" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
       </c>
       <c r="C10" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7">
         <v>77.5</v>
@@ -2187,20 +2170,19 @@
       <c r="G10" s="7">
         <v>13</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" t="s" s="8">
-        <v>26</v>
+      <c r="H10" t="s" s="8">
+        <v>25</v>
       </c>
     </row>
     <row r="11" ht="27" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
       </c>
       <c r="C11" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="7">
         <v>200</v>
@@ -2214,20 +2196,19 @@
       <c r="G11" s="7">
         <v>24.5</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" t="s" s="8">
-        <v>12</v>
+      <c r="H11" t="s" s="8">
+        <v>11</v>
       </c>
     </row>
     <row r="12" ht="27" customHeight="1">
-      <c r="A12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="B12" s="11">
+      <c r="A12" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10">
         <v>1.5</v>
       </c>
       <c r="C12" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="7">
         <v>280</v>
@@ -2241,20 +2222,19 @@
       <c r="G12" s="7">
         <v>42</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" t="s" s="8">
-        <v>20</v>
+      <c r="H12" t="s" s="8">
+        <v>19</v>
       </c>
     </row>
     <row r="13" ht="12.7" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="7">
         <v>1</v>
       </c>
       <c r="C13" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="7">
         <v>110</v>
@@ -2263,25 +2243,24 @@
         <v>2</v>
       </c>
       <c r="F13" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="7">
         <v>25</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" t="s" s="8">
-        <v>30</v>
+      <c r="H13" t="s" s="8">
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="27" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7">
         <v>1</v>
       </c>
       <c r="C14" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="7">
         <v>185</v>
@@ -2295,62 +2274,59 @@
       <c r="G14" s="7">
         <v>31</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" t="s" s="8">
-        <v>30</v>
+      <c r="H14" t="s" s="8">
+        <v>29</v>
       </c>
     </row>
     <row r="15" ht="12.7" customHeight="1">
       <c r="A15" t="s" s="6">
+        <v>31</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s" s="8">
         <v>32</v>
-      </c>
-      <c r="B15" s="7">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s" s="8">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" t="s" s="8">
-        <v>33</v>
       </c>
     </row>
     <row r="16" ht="12.7" customHeight="1">
       <c r="A16" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s" s="8">
         <v>34</v>
       </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9"/>
       <c r="D16" s="7">
         <v>190</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" s="7">
         <v>30</v>
       </c>
-      <c r="H16" s="12">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s" s="8">
+      <c r="H16" t="s" s="8">
         <v>35</v>
       </c>
     </row>
@@ -2361,7 +2337,9 @@
       <c r="B17" s="7">
         <v>1</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" t="s" s="8">
+        <v>34</v>
+      </c>
       <c r="D17" s="7">
         <v>95</v>
       </c>
@@ -2369,15 +2347,12 @@
         <v>2</v>
       </c>
       <c r="F17" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="7">
         <v>4</v>
       </c>
-      <c r="H17" s="12">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s" s="8">
+      <c r="H17" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -2388,7 +2363,9 @@
       <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" t="s" s="8">
+        <v>34</v>
+      </c>
       <c r="D18" s="7">
         <v>185</v>
       </c>
@@ -2401,10 +2378,7 @@
       <c r="G18" s="7">
         <v>16</v>
       </c>
-      <c r="H18" s="12">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s" s="8">
+      <c r="H18" t="s" s="8">
         <v>39</v>
       </c>
     </row>
@@ -2415,36 +2389,34 @@
       <c r="B19" s="7">
         <v>1</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" t="s" s="8">
+        <v>34</v>
+      </c>
       <c r="D19" s="7">
         <v>165</v>
       </c>
       <c r="E19" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" s="7">
         <v>23.75</v>
       </c>
-      <c r="H19" s="12">
-        <v>10</v>
-      </c>
-      <c r="I19" t="s" s="8">
+      <c r="H19" t="s" s="8">
         <v>41</v>
       </c>
     </row>
     <row r="20" ht="12.7" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2457,16 +2429,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.8516" style="14" customWidth="1"/>
-    <col min="2" max="8" width="10.8516" style="14" customWidth="1"/>
-    <col min="9" max="9" width="25.1719" style="14" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="14" customWidth="1"/>
+    <col min="1" max="1" width="22.8516" style="12" customWidth="1"/>
+    <col min="2" max="7" width="10.8516" style="12" customWidth="1"/>
+    <col min="8" max="8" width="25.1719" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="10.8516" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="92" customHeight="1">
@@ -2494,45 +2466,40 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" ht="12.7" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" ht="26" customHeight="1">
       <c r="A3" t="s" s="6">
         <v>42</v>
       </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s" s="17">
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="16">
         <v>43</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>260</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>11</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>8</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>37</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" t="s" s="19">
+      <c r="H3" t="s" s="18">
         <v>44</v>
       </c>
     </row>
@@ -2540,53 +2507,51 @@
       <c r="A4" t="s" s="6">
         <v>45</v>
       </c>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="17">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="16">
         <v>46</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>135</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>4.5</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>4</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>21</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" t="s" s="19">
+      <c r="H4" t="s" s="18">
         <v>47</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1">
-      <c r="A5" t="s" s="10">
+      <c r="A5" t="s" s="9">
         <v>48</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" t="s" s="17">
+      <c r="C5" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>270</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>4</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>10</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <v>40</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" t="s" s="19">
+      <c r="H5" t="s" s="18">
         <v>50</v>
       </c>
     </row>
@@ -2594,26 +2559,25 @@
       <c r="A6" t="s" s="6">
         <v>51</v>
       </c>
-      <c r="B6" s="12">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s" s="17">
+      <c r="B6" s="15">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>270</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>11</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>8</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <v>39.5</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" t="s" s="19">
+      <c r="H6" t="s" s="18">
         <v>53</v>
       </c>
     </row>
@@ -2621,107 +2585,103 @@
       <c r="A7" t="s" s="6">
         <v>54</v>
       </c>
-      <c r="B7" s="12">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s" s="17">
+      <c r="B7" s="15">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="16">
         <v>55</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>270</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <v>4</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>10</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <v>40</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" t="s" s="19">
+      <c r="H7" t="s" s="18">
         <v>56</v>
       </c>
     </row>
     <row r="8" ht="26" customHeight="1">
-      <c r="A8" t="s" s="10">
+      <c r="A8" t="s" s="9">
         <v>57</v>
       </c>
-      <c r="B8" s="12">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s" s="17">
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>110</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>8</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>7.5</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>2</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" t="s" s="19">
+      <c r="H8" t="s" s="18">
         <v>59</v>
       </c>
     </row>
     <row r="9" ht="26" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="A9" t="s" s="9">
         <v>60</v>
       </c>
-      <c r="B9" s="12">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s" s="17">
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>157.5</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>10.5</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>12.5</v>
       </c>
-      <c r="G9" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" t="s" s="19">
+      <c r="G9" t="s" s="18">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s" s="18">
         <v>61</v>
       </c>
     </row>
     <row r="10" ht="27" customHeight="1">
-      <c r="A10" t="s" s="10">
+      <c r="A10" t="s" s="9">
         <v>62</v>
       </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="17">
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>218.75</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>9.5</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>12.5</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>16</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" t="s" s="19">
+      <c r="H10" t="s" s="18">
         <v>63</v>
       </c>
     </row>
@@ -2729,86 +2689,83 @@
       <c r="A11" t="s" s="6">
         <v>64</v>
       </c>
-      <c r="B11" s="12">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s" s="17">
+      <c r="B11" s="15">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>157.5</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>11</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>8</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>10</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" t="s" s="19">
+      <c r="H11" t="s" s="18">
         <v>65</v>
       </c>
     </row>
     <row r="12" ht="26" customHeight="1">
-      <c r="A12" t="s" s="10">
+      <c r="A12" t="s" s="9">
         <v>66</v>
       </c>
-      <c r="B12" s="12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="17">
+      <c r="B12" s="15">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>125</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>10.5</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>9</v>
       </c>
-      <c r="G12" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" t="s" s="19">
+      <c r="G12" t="s" s="18">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s" s="18">
         <v>67</v>
       </c>
     </row>
     <row r="13" ht="27" customHeight="1">
-      <c r="A13" t="s" s="10">
+      <c r="A13" t="s" s="9">
         <v>68</v>
       </c>
-      <c r="B13" s="12">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="17">
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s" s="16">
         <v>46</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>270</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>9.5</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>10</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <v>34</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" t="s" s="19">
+      <c r="H13" t="s" s="18">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2820,16 +2777,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.8516" style="20" customWidth="1"/>
-    <col min="2" max="8" width="10.8516" style="20" customWidth="1"/>
-    <col min="9" max="9" width="25.1719" style="20" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="20" customWidth="1"/>
+    <col min="1" max="1" width="22.8516" style="19" customWidth="1"/>
+    <col min="2" max="7" width="10.8516" style="19" customWidth="1"/>
+    <col min="8" max="8" width="25.1719" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="10.8516" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="92" customHeight="1">
@@ -2857,45 +2814,40 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" ht="12.7" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
     </row>
     <row r="3" ht="26" customHeight="1">
       <c r="A3" t="s" s="6">
         <v>70</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.75</v>
       </c>
-      <c r="C3" t="s" s="19">
+      <c r="C3" t="s" s="18">
         <v>71</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>142.5</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>8</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>3.5</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>20</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" t="s" s="17">
+      <c r="H3" t="s" s="16">
         <v>72</v>
       </c>
     </row>
@@ -2903,80 +2855,77 @@
       <c r="A4" t="s" s="6">
         <v>73</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.5</v>
       </c>
-      <c r="C4" t="s" s="19">
+      <c r="C4" t="s" s="18">
         <v>74</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>187.5</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>8</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>8.5</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>20</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" t="s" s="17">
+      <c r="H4" t="s" s="16">
         <v>72</v>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
-      <c r="A5" t="s" s="10">
+      <c r="A5" t="s" s="9">
         <v>75</v>
       </c>
-      <c r="B5" s="12">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s" s="19">
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s" s="18">
         <v>76</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>372.5</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>23.5</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>16.5</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <v>20</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" t="s" s="17">
+      <c r="H5" t="s" s="16">
         <v>77</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="10">
+      <c r="A6" t="s" s="9">
         <v>78</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.5</v>
       </c>
-      <c r="C6" t="s" s="19">
+      <c r="C6" t="s" s="18">
         <v>79</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>25</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>2</v>
       </c>
-      <c r="F6" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="F6" t="s" s="18">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17">
         <v>20</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" t="s" s="17">
+      <c r="H6" t="s" s="16">
         <v>69</v>
       </c>
     </row>
@@ -2984,107 +2933,103 @@
       <c r="A7" t="s" s="6">
         <v>80</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.5</v>
       </c>
-      <c r="C7" t="s" s="19">
+      <c r="C7" t="s" s="18">
         <v>71</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>47.5</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <v>2</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>2.5</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <v>4</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" t="s" s="17">
+      <c r="H7" t="s" s="16">
         <v>69</v>
       </c>
     </row>
     <row r="8" ht="26" customHeight="1">
-      <c r="A8" t="s" s="10">
+      <c r="A8" t="s" s="9">
         <v>81</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.5</v>
       </c>
-      <c r="C8" t="s" s="19">
+      <c r="C8" t="s" s="18">
         <v>76</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>70</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>2</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>5</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>4</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" t="s" s="17">
+      <c r="H8" t="s" s="16">
         <v>69</v>
       </c>
     </row>
     <row r="9" ht="27" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="A9" t="s" s="9">
         <v>82</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.5</v>
       </c>
-      <c r="C9" t="s" s="19">
+      <c r="C9" t="s" s="18">
         <v>71</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>92.5</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>2</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>7.5</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <v>4</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" t="s" s="17">
+      <c r="H9" t="s" s="16">
         <v>69</v>
       </c>
     </row>
     <row r="10" ht="26" customHeight="1">
-      <c r="A10" t="s" s="10">
+      <c r="A10" t="s" s="9">
         <v>83</v>
       </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="19">
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="18">
         <v>84</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>97.5</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>6.5</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>5</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>6</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" t="s" s="17">
+      <c r="H10" t="s" s="16">
         <v>85</v>
       </c>
     </row>
@@ -3092,194 +3037,187 @@
       <c r="A11" t="s" s="6">
         <v>86</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.5</v>
       </c>
-      <c r="C11" t="s" s="19">
+      <c r="C11" t="s" s="18">
         <v>87</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>145</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>9</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>10</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>4</v>
       </c>
-      <c r="H11" s="26"/>
-      <c r="I11" t="s" s="17">
+      <c r="H11" t="s" s="16">
         <v>69</v>
       </c>
     </row>
     <row r="12" ht="26" customHeight="1">
-      <c r="A12" t="s" s="10">
+      <c r="A12" t="s" s="9">
         <v>88</v>
       </c>
-      <c r="B12" s="12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="19">
+      <c r="B12" s="15">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="18">
         <v>87</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>170</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>6</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>12.5</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>7.75</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" t="s" s="17">
+      <c r="H12" t="s" s="16">
         <v>85</v>
       </c>
     </row>
     <row r="13" ht="26" customHeight="1">
-      <c r="A13" t="s" s="10">
+      <c r="A13" t="s" s="9">
         <v>89</v>
       </c>
-      <c r="B13" s="12">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="19">
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s" s="18">
         <v>90</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>70</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>5</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <v>4</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" t="s" s="17">
+      <c r="H13" t="s" s="16">
         <v>69</v>
       </c>
     </row>
     <row r="14" ht="32" customHeight="1">
-      <c r="A14" t="s" s="10">
+      <c r="A14" t="s" s="9">
         <v>91</v>
       </c>
-      <c r="B14" s="25">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="27">
+      <c r="B14" s="24">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="25">
         <v>76</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>217.5</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="26">
         <v>13.5</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="26">
         <v>15</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="26">
         <v>6</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" t="s" s="30">
+      <c r="H14" t="s" s="27">
         <v>85</v>
       </c>
     </row>
     <row r="15" ht="32" customHeight="1">
-      <c r="A15" t="s" s="10">
+      <c r="A15" t="s" s="9">
         <v>92</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.5</v>
       </c>
-      <c r="C15" t="s" s="27">
+      <c r="C15" t="s" s="25">
         <v>93</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>122.5</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="26">
         <v>2</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="26">
         <v>7.5</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="26">
         <v>11.5</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" t="s" s="30">
+      <c r="H15" t="s" s="27">
         <v>69</v>
       </c>
     </row>
     <row r="16" ht="32" customHeight="1">
-      <c r="A16" t="s" s="10">
+      <c r="A16" t="s" s="9">
         <v>94</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>0.5</v>
       </c>
-      <c r="C16" t="s" s="27">
+      <c r="C16" t="s" s="25">
         <v>95</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>150</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <v>3</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="26">
         <v>5</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="26">
         <v>22.5</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" t="s" s="30">
+      <c r="H16" t="s" s="27">
         <v>96</v>
       </c>
     </row>
     <row r="17" ht="32" customHeight="1">
-      <c r="A17" t="s" s="10">
+      <c r="A17" t="s" s="9">
         <v>97</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>0.5</v>
       </c>
-      <c r="C17" t="s" s="27">
+      <c r="C17" t="s" s="25">
         <v>76</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>185</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <v>4.25</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="26">
         <v>11.25</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="26">
         <v>16</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" t="s" s="30">
+      <c r="H17" t="s" s="27">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3291,18 +3229,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.8516" style="31" customWidth="1"/>
-    <col min="2" max="2" width="10.8516" style="31" customWidth="1"/>
-    <col min="3" max="3" width="9.67188" style="31" customWidth="1"/>
-    <col min="4" max="8" width="10.8516" style="31" customWidth="1"/>
-    <col min="9" max="9" width="25.1719" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="31" customWidth="1"/>
+    <col min="1" max="1" width="22.8516" style="28" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="28" customWidth="1"/>
+    <col min="3" max="3" width="9.67188" style="28" customWidth="1"/>
+    <col min="4" max="7" width="10.8516" style="28" customWidth="1"/>
+    <col min="8" max="8" width="25.1719" style="28" customWidth="1"/>
+    <col min="9" max="16384" width="10.8516" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="92" customHeight="1">
@@ -3330,43 +3268,40 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" ht="12.7" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" ht="27" customHeight="1">
-      <c r="A3" t="s" s="10">
+      <c r="A3" t="s" s="9">
         <v>99</v>
       </c>
-      <c r="B3" s="35">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s" s="17">
+      <c r="B3" s="32">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="33">
         <v>11.25</v>
       </c>
-      <c r="E3" t="s" s="17">
-        <v>11</v>
-      </c>
-      <c r="F3" s="36">
+      <c r="E3" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="F3" s="33">
         <v>1.25</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" t="s" s="17">
+      <c r="G3" s="32">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s" s="16">
         <v>101</v>
       </c>
     </row>
@@ -3374,188 +3309,181 @@
       <c r="A4" t="s" s="6">
         <v>102</v>
       </c>
-      <c r="B4" s="35">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="17">
+      <c r="B4" s="32">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="33">
         <v>60</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="33">
         <v>3</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="33">
         <v>2.5</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="33">
         <v>6</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" t="s" s="17">
+      <c r="H4" t="s" s="16">
         <v>103</v>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
-      <c r="A5" t="s" s="10">
+      <c r="A5" t="s" s="9">
         <v>104</v>
       </c>
-      <c r="B5" s="35">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s" s="17">
+      <c r="B5" s="32">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="33">
         <v>97</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="33">
         <v>4.97</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="33">
         <v>5.14</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="33">
         <v>7.96</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" t="s" s="17">
+      <c r="H5" t="s" s="16">
         <v>105</v>
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
-      <c r="A6" t="s" s="10">
+      <c r="A6" t="s" s="9">
         <v>106</v>
       </c>
-      <c r="B6" s="35">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s" s="17">
+      <c r="B6" s="32">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="33">
         <v>98.78</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="33">
         <v>2.5</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="33">
         <v>2.5</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="33">
         <v>16</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" t="s" s="17">
+      <c r="H6" t="s" s="16">
         <v>98</v>
       </c>
     </row>
     <row r="7" ht="26" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="A7" t="s" s="9">
         <v>107</v>
       </c>
-      <c r="B7" s="35">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s" s="17">
+      <c r="B7" s="32">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="33">
         <v>87.5</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="33">
         <v>2.5</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="33">
         <v>2.5</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="33">
         <v>13.25</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" t="s" s="17">
+      <c r="H7" t="s" s="16">
         <v>108</v>
       </c>
     </row>
     <row r="8" ht="26" customHeight="1">
-      <c r="A8" t="s" s="10">
+      <c r="A8" t="s" s="9">
         <v>109</v>
       </c>
-      <c r="B8" s="35">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s" s="17">
+      <c r="B8" s="32">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="33">
         <v>150</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="33">
         <v>6</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="33">
         <v>6.5</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="33">
         <v>17.25</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" t="s" s="17">
+      <c r="H8" t="s" s="16">
         <v>110</v>
       </c>
     </row>
     <row r="9" ht="26" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="A9" t="s" s="9">
         <v>111</v>
       </c>
-      <c r="B9" s="35">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s" s="17">
+      <c r="B9" s="32">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="33">
         <v>141.25</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="33">
         <v>6.5</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="33">
         <v>5.75</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="33">
         <v>16</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" t="s" s="17">
+      <c r="H9" t="s" s="16">
         <v>98</v>
       </c>
     </row>
     <row r="10" ht="26" customHeight="1">
-      <c r="A10" t="s" s="10">
+      <c r="A10" t="s" s="9">
         <v>112</v>
       </c>
-      <c r="B10" s="35">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="17">
+      <c r="B10" s="32">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="33">
         <v>51.25</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="33">
         <v>4.5</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="33">
         <v>2.75</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="33">
         <v>2</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" t="s" s="17">
+      <c r="H10" t="s" s="16">
         <v>108</v>
       </c>
     </row>
@@ -3563,128 +3491,135 @@
       <c r="A11" t="s" s="6">
         <v>113</v>
       </c>
-      <c r="B11" s="35">
-        <v>1</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="35"/>
+      <c r="B11" s="32">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s" s="16">
+        <v>114</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s" s="16">
+        <v>114</v>
+      </c>
     </row>
     <row r="12" ht="26" customHeight="1">
-      <c r="A12" t="s" s="10">
-        <v>114</v>
-      </c>
-      <c r="B12" s="35">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="17">
+      <c r="A12" t="s" s="9">
         <v>115</v>
       </c>
-      <c r="D12" s="36">
+      <c r="B12" s="32">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="16">
+        <v>116</v>
+      </c>
+      <c r="D12" s="33">
         <v>168.75</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="33">
         <v>4.5</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="33">
         <v>2.5</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="33">
         <v>31</v>
       </c>
-      <c r="H12" s="36"/>
-      <c r="I12" t="s" s="17">
+      <c r="H12" t="s" s="16">
         <v>50</v>
       </c>
     </row>
     <row r="13" ht="27" customHeight="1">
-      <c r="A13" t="s" s="10">
+      <c r="A13" t="s" s="9">
+        <v>117</v>
+      </c>
+      <c r="B13" s="32">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s" s="16">
         <v>116</v>
       </c>
-      <c r="B13" s="35">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="17">
-        <v>115</v>
-      </c>
-      <c r="D13" s="36">
+      <c r="D13" s="33">
         <v>175</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="33">
         <v>5</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="33">
         <v>2.5</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="33">
         <v>32</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" t="s" s="17">
-        <v>117</v>
+      <c r="H13" t="s" s="16">
+        <v>118</v>
       </c>
     </row>
     <row r="14" ht="27" customHeight="1">
-      <c r="A14" t="s" s="10">
-        <v>118</v>
-      </c>
-      <c r="B14" s="35">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="17">
+      <c r="A14" t="s" s="9">
         <v>119</v>
       </c>
-      <c r="D14" s="37">
+      <c r="B14" s="32">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="16">
+        <v>120</v>
+      </c>
+      <c r="D14" s="34">
         <v>282.5</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="34">
         <v>11</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="34">
         <v>12.5</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="34">
         <v>30</v>
       </c>
-      <c r="H14" s="37"/>
-      <c r="I14" t="s" s="30">
+      <c r="H14" t="s" s="27">
         <v>50</v>
       </c>
     </row>
     <row r="15" ht="32" customHeight="1">
-      <c r="A15" t="s" s="10">
+      <c r="A15" t="s" s="9">
+        <v>121</v>
+      </c>
+      <c r="B15" s="32">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s" s="16">
         <v>120</v>
       </c>
-      <c r="B15" s="35">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s" s="17">
-        <v>119</v>
-      </c>
-      <c r="D15" s="37">
+      <c r="D15" s="34">
         <v>207.5</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="34">
         <v>4</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="34">
         <v>7.5</v>
       </c>
-      <c r="G15" s="37">
+      <c r="G15" s="34">
         <v>30</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" t="s" s="30">
-        <v>121</v>
+      <c r="H15" t="s" s="27">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3696,18 +3631,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.8516" style="38" customWidth="1"/>
-    <col min="2" max="2" width="10.8516" style="38" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="38" customWidth="1"/>
-    <col min="4" max="8" width="10.8516" style="38" customWidth="1"/>
-    <col min="9" max="9" width="25.1719" style="38" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="38" customWidth="1"/>
+    <col min="1" max="1" width="22.8516" style="35" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="35" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="35" customWidth="1"/>
+    <col min="4" max="7" width="10.8516" style="35" customWidth="1"/>
+    <col min="8" max="8" width="25.1719" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="10.8516" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="92" customHeight="1">
@@ -3735,344 +3670,332 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" ht="12.7" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" ht="27" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>122</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s" s="17">
+      <c r="A3" t="s" s="9">
         <v>123</v>
       </c>
-      <c r="D3" s="18">
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="16">
+        <v>124</v>
+      </c>
+      <c r="D3" s="17">
         <v>247.5</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>21</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>17.5</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="26"/>
-      <c r="I3" t="s" s="19">
-        <v>124</v>
+      <c r="G3" s="17">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s" s="18">
+        <v>125</v>
       </c>
     </row>
     <row r="4" ht="27" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="A4" t="s" s="9">
+        <v>126</v>
+      </c>
+      <c r="B4" s="15">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s" s="18">
+        <v>127</v>
+      </c>
+      <c r="D4" s="17">
+        <v>282.5</v>
+      </c>
+      <c r="E4" s="17">
+        <v>22</v>
+      </c>
+      <c r="F4" s="17">
+        <v>20</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s" s="18">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" ht="27" customHeight="1">
+      <c r="A5" t="s" s="9">
+        <v>128</v>
+      </c>
+      <c r="B5" s="15">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s" s="18">
+        <v>127</v>
+      </c>
+      <c r="D5" s="17">
+        <v>270</v>
+      </c>
+      <c r="E5" s="17">
+        <v>21</v>
+      </c>
+      <c r="F5" s="17">
+        <v>20</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s" s="18">
         <v>125</v>
       </c>
-      <c r="B4" s="12">
+    </row>
+    <row r="6" ht="27" customHeight="1">
+      <c r="A6" t="s" s="9">
+        <v>129</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="C6" t="s" s="16">
+        <v>130</v>
+      </c>
+      <c r="D6" s="17">
+        <v>247.5</v>
+      </c>
+      <c r="E6" s="17">
+        <v>20.5</v>
+      </c>
+      <c r="F6" s="17">
+        <v>15</v>
+      </c>
+      <c r="G6" s="17">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s" s="18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" ht="40" customHeight="1">
+      <c r="A7" t="s" s="9">
+        <v>132</v>
+      </c>
+      <c r="B7" s="15">
         <v>100</v>
       </c>
-      <c r="C4" t="s" s="19">
-        <v>126</v>
-      </c>
-      <c r="D4" s="18">
-        <v>282.5</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="C7" t="s" s="18">
+        <v>127</v>
+      </c>
+      <c r="D7" s="17">
+        <v>352.5</v>
+      </c>
+      <c r="E7" s="17">
+        <v>18.5</v>
+      </c>
+      <c r="F7" s="17">
+        <v>25</v>
+      </c>
+      <c r="G7" s="17">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s" s="18">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" ht="26" customHeight="1">
+      <c r="A8" t="s" s="9">
+        <v>134</v>
+      </c>
+      <c r="B8" s="15">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s" s="18">
+        <v>127</v>
+      </c>
+      <c r="D8" s="17">
+        <v>350</v>
+      </c>
+      <c r="E8" s="17">
         <v>22</v>
       </c>
-      <c r="F4" s="18">
-        <v>20</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="F8" s="17">
+        <v>25</v>
+      </c>
+      <c r="G8" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="H8" t="s" s="18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" ht="27" customHeight="1">
+      <c r="A9" t="s" s="9">
+        <v>136</v>
+      </c>
+      <c r="B9" s="15">
+        <v>150</v>
+      </c>
+      <c r="C9" t="s" s="18">
+        <v>127</v>
+      </c>
+      <c r="D9" s="17">
+        <v>332.5</v>
+      </c>
+      <c r="E9" s="17">
+        <v>15.5</v>
+      </c>
+      <c r="F9" s="17">
+        <v>15</v>
+      </c>
+      <c r="G9" s="17">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s" s="18">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" ht="26" customHeight="1">
+      <c r="A10" t="s" s="9">
+        <v>137</v>
+      </c>
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="18">
+        <v>138</v>
+      </c>
+      <c r="D10" s="17">
+        <v>365</v>
+      </c>
+      <c r="E10" s="17">
+        <v>14</v>
+      </c>
+      <c r="F10" s="17">
+        <v>12.5</v>
+      </c>
+      <c r="G10" s="17">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s" s="18">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" ht="26" customHeight="1">
+      <c r="A11" t="s" s="9">
+        <v>139</v>
+      </c>
+      <c r="B11" s="15">
+        <v>150</v>
+      </c>
+      <c r="C11" t="s" s="18">
+        <v>127</v>
+      </c>
+      <c r="D11" s="17">
+        <v>240</v>
+      </c>
+      <c r="E11" s="17">
+        <v>13</v>
+      </c>
+      <c r="F11" s="17">
+        <v>5</v>
+      </c>
+      <c r="G11" s="17">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s" s="18">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" ht="27" customHeight="1">
+      <c r="A12" t="s" s="9">
+        <v>141</v>
+      </c>
+      <c r="B12" s="15">
         <v>2</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" t="s" s="19">
+      <c r="C12" t="s" s="18">
+        <v>142</v>
+      </c>
+      <c r="D12" s="17">
+        <v>380</v>
+      </c>
+      <c r="E12" s="17">
+        <v>19</v>
+      </c>
+      <c r="F12" s="17">
+        <v>11</v>
+      </c>
+      <c r="G12" s="17">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s" s="18">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" ht="26" customHeight="1">
+      <c r="A13" t="s" s="9">
+        <v>144</v>
+      </c>
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s" s="16">
+        <v>145</v>
+      </c>
+      <c r="D13" s="17">
+        <v>240</v>
+      </c>
+      <c r="E13" s="17">
+        <v>13</v>
+      </c>
+      <c r="F13" s="17">
+        <v>5</v>
+      </c>
+      <c r="G13" s="17">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s" s="18">
         <v>59</v>
       </c>
     </row>
-    <row r="5" ht="27" customHeight="1">
-      <c r="A5" t="s" s="10">
-        <v>127</v>
-      </c>
-      <c r="B5" s="12">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s" s="19">
-        <v>126</v>
-      </c>
-      <c r="D5" s="18">
-        <v>270</v>
-      </c>
-      <c r="E5" s="18">
-        <v>21</v>
-      </c>
-      <c r="F5" s="18">
-        <v>20</v>
-      </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="26"/>
-      <c r="I5" t="s" s="19">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" ht="27" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>128</v>
-      </c>
-      <c r="B6" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="C6" t="s" s="17">
-        <v>129</v>
-      </c>
-      <c r="D6" s="18">
-        <v>247.5</v>
-      </c>
-      <c r="E6" s="18">
-        <v>20.5</v>
-      </c>
-      <c r="F6" s="18">
-        <v>15</v>
-      </c>
-      <c r="G6" s="18">
-        <v>6</v>
-      </c>
-      <c r="H6" s="26"/>
-      <c r="I6" t="s" s="19">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" ht="40" customHeight="1">
-      <c r="A7" t="s" s="10">
-        <v>131</v>
-      </c>
-      <c r="B7" s="12">
-        <v>100</v>
-      </c>
-      <c r="C7" t="s" s="19">
-        <v>126</v>
-      </c>
-      <c r="D7" s="18">
-        <v>352.5</v>
-      </c>
-      <c r="E7" s="18">
-        <v>18.5</v>
-      </c>
-      <c r="F7" s="18">
-        <v>25</v>
-      </c>
-      <c r="G7" s="18">
-        <v>12</v>
-      </c>
-      <c r="H7" s="26"/>
-      <c r="I7" t="s" s="19">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" ht="26" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>133</v>
-      </c>
-      <c r="B8" s="12">
-        <v>100</v>
-      </c>
-      <c r="C8" t="s" s="19">
-        <v>126</v>
-      </c>
-      <c r="D8" s="18">
-        <v>350</v>
-      </c>
-      <c r="E8" s="18">
-        <v>22</v>
-      </c>
-      <c r="F8" s="18">
-        <v>25</v>
-      </c>
-      <c r="G8" s="18">
-        <v>7.5</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" t="s" s="19">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" ht="27" customHeight="1">
-      <c r="A9" t="s" s="10">
-        <v>135</v>
-      </c>
-      <c r="B9" s="12">
-        <v>150</v>
-      </c>
-      <c r="C9" t="s" s="19">
-        <v>126</v>
-      </c>
-      <c r="D9" s="18">
-        <v>332.5</v>
-      </c>
-      <c r="E9" s="18">
-        <v>15.5</v>
-      </c>
-      <c r="F9" s="18">
-        <v>15</v>
-      </c>
-      <c r="G9" s="18">
+    <row r="14" ht="26" customHeight="1">
+      <c r="A14" t="s" s="9">
+        <v>146</v>
+      </c>
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="16">
+        <v>145</v>
+      </c>
+      <c r="D14" s="17">
+        <v>327.5</v>
+      </c>
+      <c r="E14" s="17">
+        <v>23.5</v>
+      </c>
+      <c r="F14" s="17">
+        <v>11</v>
+      </c>
+      <c r="G14" s="17">
         <v>32</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" t="s" s="19">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" ht="26" customHeight="1">
-      <c r="A10" t="s" s="10">
-        <v>136</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="19">
-        <v>137</v>
-      </c>
-      <c r="D10" s="18">
-        <v>365</v>
-      </c>
-      <c r="E10" s="18">
-        <v>14</v>
-      </c>
-      <c r="F10" s="18">
-        <v>12.5</v>
-      </c>
-      <c r="G10" s="18">
-        <v>47</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="I10" t="s" s="19">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" ht="26" customHeight="1">
-      <c r="A11" t="s" s="10">
-        <v>138</v>
-      </c>
-      <c r="B11" s="12">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s" s="19">
-        <v>126</v>
-      </c>
-      <c r="D11" s="18">
-        <v>240</v>
-      </c>
-      <c r="E11" s="18">
-        <v>13</v>
-      </c>
-      <c r="F11" s="18">
-        <v>5</v>
-      </c>
-      <c r="G11" s="18">
-        <v>34</v>
-      </c>
-      <c r="H11" s="26"/>
-      <c r="I11" t="s" s="19">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" ht="27" customHeight="1">
-      <c r="A12" t="s" s="10">
-        <v>140</v>
-      </c>
-      <c r="B12" s="12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s" s="19">
-        <v>141</v>
-      </c>
-      <c r="D12" s="18">
-        <v>380</v>
-      </c>
-      <c r="E12" s="18">
-        <v>19</v>
-      </c>
-      <c r="F12" s="18">
-        <v>11</v>
-      </c>
-      <c r="G12" s="18">
-        <v>50</v>
-      </c>
-      <c r="H12" s="26"/>
-      <c r="I12" t="s" s="19">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" ht="26" customHeight="1">
-      <c r="A13" t="s" s="10">
-        <v>143</v>
-      </c>
-      <c r="B13" s="12">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="17">
-        <v>144</v>
-      </c>
-      <c r="D13" s="18">
-        <v>240</v>
-      </c>
-      <c r="E13" s="18">
-        <v>13</v>
-      </c>
-      <c r="F13" s="18">
-        <v>5</v>
-      </c>
-      <c r="G13" s="18">
-        <v>34</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" t="s" s="19">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" ht="26" customHeight="1">
-      <c r="A14" t="s" s="10">
-        <v>145</v>
-      </c>
-      <c r="B14" s="12">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="17">
-        <v>144</v>
-      </c>
-      <c r="D14" s="18">
-        <v>327.5</v>
-      </c>
-      <c r="E14" s="18">
-        <v>23.5</v>
-      </c>
-      <c r="F14" s="18">
-        <v>11</v>
-      </c>
-      <c r="G14" s="18">
-        <v>32</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" t="s" s="19">
+      <c r="H14" t="s" s="18">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -4084,18 +4007,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.8516" style="42" customWidth="1"/>
-    <col min="2" max="6" width="10.8516" style="42" customWidth="1"/>
-    <col min="7" max="7" width="28.3203" style="42" customWidth="1"/>
-    <col min="8" max="8" width="10.8516" style="42" customWidth="1"/>
-    <col min="9" max="9" width="25.1719" style="42" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="42" customWidth="1"/>
+    <col min="1" max="1" width="22.8516" style="39" customWidth="1"/>
+    <col min="2" max="6" width="10.8516" style="39" customWidth="1"/>
+    <col min="7" max="7" width="28.3516" style="39" customWidth="1"/>
+    <col min="8" max="8" width="25.1719" style="39" customWidth="1"/>
+    <col min="9" max="16384" width="10.8516" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="92" customHeight="1">
@@ -4123,247 +4045,254 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" ht="12.7" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" ht="26" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>146</v>
-      </c>
-      <c r="B3" s="24">
+      <c r="A3" t="s" s="9">
+        <v>147</v>
+      </c>
+      <c r="B3" s="23">
         <v>0.5</v>
       </c>
-      <c r="C3" t="s" s="17">
-        <v>147</v>
-      </c>
-      <c r="D3" s="18">
+      <c r="C3" t="s" s="16">
+        <v>148</v>
+      </c>
+      <c r="D3" s="17">
         <v>100</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18">
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0</v>
+      </c>
+      <c r="G3" s="17">
         <v>25</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" t="s" s="19">
+      <c r="H3" t="s" s="18">
         <v>47</v>
       </c>
     </row>
     <row r="4" ht="27" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="A4" t="s" s="9">
+        <v>149</v>
+      </c>
+      <c r="B4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="s" s="16">
         <v>148</v>
       </c>
-      <c r="B4" s="24">
+      <c r="D4" s="17">
+        <v>125</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17">
+        <v>5</v>
+      </c>
+      <c r="G4" s="17">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s" s="18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" t="s" s="9">
+        <v>150</v>
+      </c>
+      <c r="B5" s="23">
         <v>0.5</v>
       </c>
-      <c r="C4" t="s" s="17">
-        <v>147</v>
-      </c>
-      <c r="D4" s="18">
-        <v>125</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18">
+      <c r="C5" t="s" s="16">
+        <v>148</v>
+      </c>
+      <c r="D5" s="17">
+        <v>70</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17">
+        <v>17.5</v>
+      </c>
+      <c r="H5" t="s" s="18">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" t="s" s="9">
+        <v>152</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C6" t="s" s="16">
+        <v>148</v>
+      </c>
+      <c r="D6" s="17">
+        <v>145</v>
+      </c>
+      <c r="E6" s="17">
+        <v>4.5</v>
+      </c>
+      <c r="F6" s="17">
+        <v>4</v>
+      </c>
+      <c r="G6" s="17">
+        <v>23.5</v>
+      </c>
+      <c r="H6" t="s" s="18">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" ht="26" customHeight="1">
+      <c r="A7" t="s" s="9">
+        <v>153</v>
+      </c>
+      <c r="B7" s="15">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s" s="16">
+        <v>154</v>
+      </c>
+      <c r="D7" s="17">
+        <v>195</v>
+      </c>
+      <c r="E7" s="17">
+        <v>2</v>
+      </c>
+      <c r="F7" s="17">
         <v>5</v>
       </c>
-      <c r="G4" s="18">
-        <v>20</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" t="s" s="19">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" ht="26" customHeight="1">
-      <c r="A5" t="s" s="10">
-        <v>149</v>
-      </c>
-      <c r="B5" s="24">
+      <c r="G7" s="17">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s" s="18">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" ht="27" customHeight="1">
+      <c r="A8" t="s" s="9">
+        <v>156</v>
+      </c>
+      <c r="B8" s="23">
         <v>0.5</v>
       </c>
-      <c r="C5" t="s" s="17">
-        <v>147</v>
-      </c>
-      <c r="D5" s="18">
-        <v>70</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18">
-        <v>17.5</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" t="s" s="19">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" ht="26" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>151</v>
-      </c>
-      <c r="B6" s="24">
+      <c r="C8" t="s" s="16">
+        <v>148</v>
+      </c>
+      <c r="D8" s="17">
+        <v>192.5</v>
+      </c>
+      <c r="E8" s="17">
+        <v>8</v>
+      </c>
+      <c r="F8" s="17">
+        <v>6.5</v>
+      </c>
+      <c r="G8" s="17">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s" s="18">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" ht="27" customHeight="1">
+      <c r="A9" t="s" s="9">
+        <v>158</v>
+      </c>
+      <c r="B9" t="s" s="18">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s" s="18">
+        <v>160</v>
+      </c>
+      <c r="D9" s="17">
+        <v>185</v>
+      </c>
+      <c r="E9" s="17">
+        <v>2</v>
+      </c>
+      <c r="F9" s="17">
+        <v>5</v>
+      </c>
+      <c r="G9" s="17">
+        <v>32.5</v>
+      </c>
+      <c r="H9" t="s" s="18">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" ht="12.7" customHeight="1">
+      <c r="A10" t="s" s="9">
+        <v>161</v>
+      </c>
+      <c r="B10" s="23">
         <v>0.5</v>
       </c>
-      <c r="C6" t="s" s="17">
-        <v>147</v>
-      </c>
-      <c r="D6" s="18">
-        <v>145</v>
-      </c>
-      <c r="E6" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="F6" s="18">
+      <c r="C10" t="s" s="18">
+        <v>162</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s" s="18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" ht="26" customHeight="1">
+      <c r="A11" t="s" s="9">
+        <v>163</v>
+      </c>
+      <c r="B11" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C11" t="s" s="18">
+        <v>76</v>
+      </c>
+      <c r="D11" s="17">
+        <v>185</v>
+      </c>
+      <c r="E11" s="17">
+        <v>6.5</v>
+      </c>
+      <c r="F11" s="17">
         <v>4</v>
       </c>
-      <c r="G6" s="18">
-        <v>23.5</v>
-      </c>
-      <c r="H6" s="18"/>
-      <c r="I6" t="s" s="19">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" ht="26" customHeight="1">
-      <c r="A7" t="s" s="10">
-        <v>152</v>
-      </c>
-      <c r="B7" s="12">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s" s="17">
-        <v>153</v>
-      </c>
-      <c r="D7" s="18">
-        <v>195</v>
-      </c>
-      <c r="E7" s="18">
-        <v>2</v>
-      </c>
-      <c r="F7" s="18">
-        <v>5</v>
-      </c>
-      <c r="G7" s="18">
-        <v>35</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" t="s" s="19">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" ht="27" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>155</v>
-      </c>
-      <c r="B8" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="C8" t="s" s="17">
-        <v>147</v>
-      </c>
-      <c r="D8" s="18">
-        <v>192.5</v>
-      </c>
-      <c r="E8" s="18">
-        <v>8</v>
-      </c>
-      <c r="F8" s="18">
-        <v>6.5</v>
-      </c>
-      <c r="G8" s="18">
-        <v>26</v>
-      </c>
-      <c r="H8" s="18"/>
-      <c r="I8" t="s" s="19">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" ht="27" customHeight="1">
-      <c r="A9" t="s" s="10">
-        <v>157</v>
-      </c>
-      <c r="B9" t="s" s="19">
-        <v>158</v>
-      </c>
-      <c r="C9" t="s" s="19">
-        <v>159</v>
-      </c>
-      <c r="D9" s="18">
-        <v>185</v>
-      </c>
-      <c r="E9" s="18">
-        <v>2</v>
-      </c>
-      <c r="F9" s="18">
-        <v>5</v>
-      </c>
-      <c r="G9" s="18">
-        <v>32.5</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" t="s" s="19">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" ht="12.7" customHeight="1">
-      <c r="A10" t="s" s="10">
-        <v>160</v>
-      </c>
-      <c r="B10" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="C10" t="s" s="19">
-        <v>161</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" ht="26" customHeight="1">
-      <c r="A11" t="s" s="10">
-        <v>162</v>
-      </c>
-      <c r="B11" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="C11" t="s" s="19">
-        <v>76</v>
-      </c>
-      <c r="D11" s="18">
-        <v>185</v>
-      </c>
-      <c r="E11" s="18">
-        <v>6.5</v>
-      </c>
-      <c r="F11" s="18">
-        <v>4</v>
-      </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>31</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" t="s" s="19">
+      <c r="H11" t="s" s="18">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>